<commit_message>
Cadena de Custodia subida / actualizada
</commit_message>
<xml_diff>
--- a/AF-P09-G3/Anexos/Anexo 2 - Registro de cadena de custodia.xlsx
+++ b/AF-P09-G3/Anexos/Anexo 2 - Registro de cadena de custodia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3kxhoDark\Desktop\CIBER\Repositorios\G3-ANALISIS-FORENSE\AF-P05-G3\Anexos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3kxhoDark\Desktop\CIBER\Repositorios\G3-ANALISIS-FORENSE\AF-P09-G3\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB700B-9061-486C-9CB8-E52EC07649F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3408DF4-6359-49E2-B741-FFA4938F0239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,10 +63,10 @@
     <t>Juan Manuel Cumbrera López</t>
   </si>
   <si>
-    <t>Lunes 15 de Abril de 2024</t>
-  </si>
-  <si>
-    <t>Elaboración de un informe técnico sobre el volcado de memoria y la imagen del disco del servidor corporativo comprometido.</t>
+    <t>Elaboración de un informe técnico sobre las capturas del tráfico de red del SmartHome, la imagen del disco del Raspberry Pi, el informe de diagnóstico de Google OnHub, los datos de Amazon Echo Alexa y  las adquisiciones de los dispositivos móviles de la víctima y de su marido.</t>
+  </si>
+  <si>
+    <t>Lunes 6 de Mayo de 2024</t>
   </si>
 </sst>
 </file>
@@ -165,23 +165,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +466,7 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -480,124 +480,124 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="2:8" ht="45">
-      <c r="B8" s="5">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" ht="120">
+      <c r="B8" s="9">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="30">
-      <c r="B9" s="5"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" ht="30">
-      <c r="B10" s="5"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
     <mergeCell ref="B3:H4"/>
     <mergeCell ref="B5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>